<commit_message>
estructura de datos corregida
</commit_message>
<xml_diff>
--- a/wordix/estructurasDatosWordix.xlsx
+++ b/wordix/estructurasDatosWordix.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD7A9E6-D745-45F8-8F5A-525DD9C9E9A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="630" windowWidth="19815" windowHeight="9405"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
   <si>
     <t>//indices</t>
   </si>
@@ -58,9 +64,6 @@
   </si>
   <si>
     <t>**** SEGUIR COMPLETANDO ****</t>
-  </si>
-  <si>
-    <t>//multidimencional</t>
   </si>
   <si>
     <t>//nombre STRING</t>
@@ -187,9 +190,6 @@
     <t>"MUJER"</t>
   </si>
   <si>
-    <t>indexado</t>
-  </si>
-  <si>
     <t>"Pedro"</t>
   </si>
   <si>
@@ -209,17 +209,125 @@
   </si>
   <si>
     <t>Nico13A</t>
+  </si>
+  <si>
+    <t>USUARIO QUIERE BUSCAR JUGADOR "Pedro"</t>
+  </si>
+  <si>
+    <t>recorrido de arreglo</t>
+  </si>
+  <si>
+    <t>EMPIEZA ACA</t>
+  </si>
+  <si>
+    <t>VERIFICA SI $coleccionPartidas[$i][$nombre] == "Pedro"</t>
+  </si>
+  <si>
+    <t>SE CALCULAN LAS VICTORIAS DEPENDIENDO SI TIENE UN PUNTAJE =! 0 EN SUS PARTIDAS</t>
+  </si>
+  <si>
+    <t>CON UN SWITCH AUMENTAMOS EL ACUMULADOR DE INTENTOS QUE CORRESPONDA</t>
+  </si>
+  <si>
+    <t>jugador</t>
+  </si>
+  <si>
+    <t>partidas</t>
+  </si>
+  <si>
+    <t>puntaje</t>
+  </si>
+  <si>
+    <t>victorias</t>
+  </si>
+  <si>
+    <t>intento1</t>
+  </si>
+  <si>
+    <t>intento2</t>
+  </si>
+  <si>
+    <t>intento3</t>
+  </si>
+  <si>
+    <t>intento4</t>
+  </si>
+  <si>
+    <t>intento 5</t>
+  </si>
+  <si>
+    <t>intento6</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$resumenJugador </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+  </si>
+  <si>
+    <t>informacion de la estructura:</t>
+  </si>
+  <si>
+    <t>Tipo de datos: Almacena valores String e INT</t>
+  </si>
+  <si>
+    <t>Para que se utiliza? Almacena un registro de cada jugador.</t>
+  </si>
+  <si>
+    <t>Tipo: Asociativo</t>
+  </si>
+  <si>
+    <t>SI ES ASI GUARDA SE CREA UN ARREGLO $resumenJugador Y GUARDA SUS DATOS AHÍ</t>
+  </si>
+  <si>
+    <t>$partidas = $partidas + 1;</t>
+  </si>
+  <si>
+    <t>$puntaje = $puntaje + $coleccionPartidas[$i][$puntos];</t>
+  </si>
+  <si>
+    <t>// indice</t>
+  </si>
+  <si>
+    <t>// valores</t>
+  </si>
+  <si>
+    <t>Informacion de la estructura:</t>
+  </si>
+  <si>
+    <t>Tipo: Multidimencional Indexado</t>
+  </si>
+  <si>
+    <t>Para que se utiliza? Guarda las partidas de cada jugador.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -280,8 +388,58 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,8 +470,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -433,79 +615,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,6 +774,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -717,25 +979,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" customWidth="1"/>
-    <col min="10" max="26" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" thickBot="1">
@@ -751,7 +1016,7 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -762,21 +1027,21 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="27" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -785,19 +1050,19 @@
     </row>
     <row r="4" spans="1:9" ht="17.25" customHeight="1" thickBot="1">
       <c r="A4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -806,19 +1071,19 @@
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickBot="1">
       <c r="A5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -827,13 +1092,13 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1">
       <c r="A6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -842,21 +1107,21 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="22.5" customHeight="1" thickBot="1">
+    <row r="7" spans="1:9" ht="18.75" customHeight="1" thickBot="1">
       <c r="A7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>55</v>
+      <c r="D7" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -887,7 +1152,7 @@
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" thickBot="1">
       <c r="A10" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="8">
         <v>0</v>
@@ -1024,7 +1289,7 @@
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" thickBot="1">
       <c r="A19" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="14">
         <v>0</v>
@@ -1048,65 +1313,61 @@
         <v>6</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" thickBot="1">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="16"/>
+      <c r="B20" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A21" s="16"/>
+      <c r="B21" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A21" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
@@ -1133,7 +1394,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
@@ -1160,7 +1421,7 @@
         <v>16</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
@@ -1175,8 +1436,10 @@
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="38"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1185,49 +1448,337 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A26" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="35"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A27" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+    </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="50" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="51" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="52" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="53" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="54" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="55" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="56" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="57" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="58" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="59" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="60" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="61" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="62" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A62" s="1" t="s">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A32" s="2"/>
+      <c r="B32" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A33" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="23">
+        <v>0</v>
+      </c>
+      <c r="C33" s="23">
+        <v>1</v>
+      </c>
+      <c r="D33" s="23">
+        <v>2</v>
+      </c>
+      <c r="E33" s="23">
+        <v>3</v>
+      </c>
+      <c r="F33" s="23">
+        <v>4</v>
+      </c>
+      <c r="G33" s="23">
+        <v>5</v>
+      </c>
+      <c r="H33" s="23">
+        <v>6</v>
+      </c>
+      <c r="I33" s="15"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A34" s="16"/>
+      <c r="B34" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A35" s="16"/>
+      <c r="B35" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I35" s="17"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A36" s="10"/>
+      <c r="B36" s="11">
+        <v>6</v>
+      </c>
+      <c r="C36" s="11">
+        <v>4</v>
+      </c>
+      <c r="D36" s="11">
+        <v>5</v>
+      </c>
+      <c r="E36" s="11">
+        <v>2</v>
+      </c>
+      <c r="F36" s="11">
+        <v>3</v>
+      </c>
+      <c r="G36" s="11">
+        <v>1</v>
+      </c>
+      <c r="H36" s="11">
+        <v>1</v>
+      </c>
+      <c r="I36" s="15"/>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11">
+        <v>0</v>
+      </c>
+      <c r="C37" s="11">
+        <v>13</v>
+      </c>
+      <c r="D37" s="11">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" ht="15.75" customHeight="1"/>
-    <row r="64" spans="1:1" ht="15.75" customHeight="1"/>
+      <c r="E37" s="11">
+        <v>15</v>
+      </c>
+      <c r="F37" s="11">
+        <v>11</v>
+      </c>
+      <c r="G37" s="11">
+        <v>15</v>
+      </c>
+      <c r="H37" s="11">
+        <v>16</v>
+      </c>
+      <c r="I37" s="15"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A39" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="41" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A41" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B43" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="I43" s="25"/>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B44" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B45" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B46" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="49" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A49" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F49" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="G49" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H49" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="I49" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="J49" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="K49" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="L49" s="33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B50" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="29">
+        <v>15</v>
+      </c>
+      <c r="D50" s="29">
+        <v>150</v>
+      </c>
+      <c r="E50" s="29">
+        <v>12</v>
+      </c>
+      <c r="F50" s="29">
+        <v>0</v>
+      </c>
+      <c r="G50" s="29">
+        <v>6</v>
+      </c>
+      <c r="H50" s="29">
+        <v>4</v>
+      </c>
+      <c r="I50" s="29">
+        <v>0</v>
+      </c>
+      <c r="J50" s="29">
+        <v>2</v>
+      </c>
+      <c r="K50" s="29">
+        <v>0</v>
+      </c>
+      <c r="L50" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="52" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A52" s="39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A53" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A54" s="25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A55" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="57" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="58" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="59" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="60" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="61" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="62" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="63" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A63" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -2164,12 +2715,16 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:C27"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:G16"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>